<commit_message>
push fall 2021 syllabus
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Fall_2021_schedule.xlsx
+++ b/vignettes/course_docs/Fall_2021_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/cognition/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4396D2-B507-8446-A233-FCBA043ADBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F00FF2E-78DD-3B4F-97C8-EF4178819A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="1560" windowWidth="16220" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="460" windowWidth="17040" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,15 +141,6 @@
     <t>Getting started</t>
   </si>
   <si>
-    <t>What is Cognition?</t>
-  </si>
-  <si>
-    <t>Memory I</t>
-  </si>
-  <si>
-    <t>Memory II</t>
-  </si>
-  <si>
     <t>Midterm I</t>
   </si>
   <si>
@@ -165,24 +156,6 @@
     <t>W 8/25/21</t>
   </si>
   <si>
-    <t>Mental Imagery</t>
-  </si>
-  <si>
-    <t>Eugenics and Psychology</t>
-  </si>
-  <si>
-    <t>Intelligence Testing</t>
-  </si>
-  <si>
-    <t>Associations</t>
-  </si>
-  <si>
-    <t>Behaviorism</t>
-  </si>
-  <si>
-    <t>Information Processing</t>
-  </si>
-  <si>
     <t>Implicit Cognition</t>
   </si>
   <si>
@@ -244,6 +217,33 @@
   </si>
   <si>
     <t>Quiz 11</t>
+  </si>
+  <si>
+    <t>[What is Cognition?](https://www.crumplab.com/cognition/textbook/what-is-cognition.html)</t>
+  </si>
+  <si>
+    <t>[Mental Imagery](https://www.crumplab.com/cognition/textbook/mental-imagery.html)</t>
+  </si>
+  <si>
+    <t>[Eugenics and Psychology](https://www.crumplab.com/cognition/textbook/eugenics-and-psychology.html)</t>
+  </si>
+  <si>
+    <t>[Intelligence Testing](https://www.crumplab.com/cognition/textbook/intelligence-testing.html)</t>
+  </si>
+  <si>
+    <t>[Associations](https://www.crumplab.com/cognition/textbook/associations.html)</t>
+  </si>
+  <si>
+    <t>[Behaviorism](https://www.crumplab.com/cognition/textbook/behaviorism.html)</t>
+  </si>
+  <si>
+    <t>[Information Processing](https://www.crumplab.com/cognition/textbook/information-processing.html)</t>
+  </si>
+  <si>
+    <t>[Memory I](https://www.crumplab.com/cognition/textbook/memory-i.html)</t>
+  </si>
+  <si>
+    <t>[Memory II](https://www.crumplab.com/cognition/textbook/memory-ii.html)</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -600,13 +600,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -614,18 +614,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -655,7 +655,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -666,7 +666,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -674,21 +674,21 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -696,21 +696,21 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -718,18 +718,18 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -748,13 +748,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -762,21 +762,21 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -784,18 +784,18 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -806,10 +806,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -828,10 +828,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -839,7 +839,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -850,10 +850,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -861,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -872,10 +872,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -905,7 +905,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -916,10 +916,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -927,7 +927,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -951,13 +951,13 @@
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update syllabus push lecture 7
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Fall_2021_schedule.xlsx
+++ b/vignettes/course_docs/Fall_2021_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/cognition/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7C660C-113D-8D4C-B77F-CFFB9011951C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5271FB5-78F8-DB4C-B898-09EBFEDFF525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="760" windowWidth="17040" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5000" yWindow="500" windowWidth="17040" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,24 +192,6 @@
     <t>Quiz 2</t>
   </si>
   <si>
-    <t>Quiz 3</t>
-  </si>
-  <si>
-    <t>Quiz 4</t>
-  </si>
-  <si>
-    <t>Quiz 5</t>
-  </si>
-  <si>
-    <t>Quiz 6</t>
-  </si>
-  <si>
-    <t>Quiz 7</t>
-  </si>
-  <si>
-    <t>Quiz 8</t>
-  </si>
-  <si>
     <t>Quiz 9</t>
   </si>
   <si>
@@ -244,6 +226,24 @@
   </si>
   <si>
     <t>[Memory II](https://www.crumplab.com/cognition/textbook/memory-ii.html)</t>
+  </si>
+  <si>
+    <t>Quiz 3 open</t>
+  </si>
+  <si>
+    <t>Quiz 4 open</t>
+  </si>
+  <si>
+    <t>Quiz 5 open</t>
+  </si>
+  <si>
+    <t>Quiz 6 open</t>
+  </si>
+  <si>
+    <t>Quiz 7 open</t>
+  </si>
+  <si>
+    <t>Quiz 8 open</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>52</v>
@@ -625,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -674,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>53</v>
@@ -685,7 +685,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -696,10 +696,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -707,7 +704,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -718,10 +718,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -729,7 +726,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -762,10 +762,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -773,7 +770,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -784,10 +784,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -795,7 +792,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -808,9 +808,6 @@
       <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
@@ -819,6 +816,9 @@
       <c r="C22" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -830,9 +830,6 @@
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
@@ -841,6 +838,9 @@
       <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -875,7 +875,7 @@
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
         <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">

</xml_diff>